<commit_message>
User can add items by entering data into the console
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date purchased</t>
   </si>
@@ -20,19 +20,25 @@
     <t>The title</t>
   </si>
   <si>
-    <t>Costed</t>
+    <t>Bought price</t>
   </si>
   <si>
-    <t>Status</t>
+    <t>Sold Price</t>
   </si>
   <si>
-    <t>01.02.2025</t>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Is sold</t>
+  </si>
+  <si>
+    <t>01-02-2025</t>
   </si>
   <si>
     <t>Nike Dunk</t>
   </si>
   <si>
-    <t>Bought</t>
+    <t>New With Tag</t>
   </si>
 </sst>
 </file>
@@ -77,11 +83,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="15.1015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="10.21875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="12.4296875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.80078125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.63671875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="6.6328125" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
@@ -96,19 +110,31 @@
       <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>12.99</v>
+        <v>13.39</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>6</v>
+      <c r="D2" t="n" s="0">
+        <v>14.56</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F2" t="b" s="0">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto calculating profit in percents and adding it to the 6 column
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date purchased</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>Is sold</t>
+  </si>
+  <si>
+    <t>Profit</t>
   </si>
   <si>
     <t>01-02-2025</t>
@@ -83,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -95,6 +98,7 @@
     <col min="4" max="4" width="9.80078125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="13.63671875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="6.6328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="6.015625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -116,25 +120,31 @@
       <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
+      <c r="G1" t="s" s="0">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>13.39</v>
+        <v>123.99</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>14.56</v>
+        <v>139.99</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
-      <c r="F2" t="b" s="0">
+      <c r="F2" t="b">
         <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>12.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>